<commit_message>
Handling id_vim on models
</commit_message>
<xml_diff>
--- a/FA_template.xlsx
+++ b/FA_template.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Issuer / Producer</t>
   </si>
   <si>
-    <t xml:space="preserve">Usage purpose</t>
+    <t xml:space="preserve">Use purpose</t>
   </si>
   <si>
     <t xml:space="preserve">Purchase value / Production cost</t>
@@ -658,7 +658,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>